<commit_message>
update excel tables and add python files
* Update excel tables 
* Add python files (create_tables, insert_tables)
</commit_message>
<xml_diff>
--- a/soil_add_horizons.xlsx
+++ b/soil_add_horizons.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3824D8-174A-4022-B54A-ECA8E6A7D259}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
   <si>
     <t>Индекс</t>
   </si>
@@ -277,9 +276,6 @@
     <t>Признаки слитости.</t>
   </si>
   <si>
-    <t>ADD_HORIZON_ID</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -295,7 +291,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -662,20 +658,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194BCD77-5A7B-4BEC-8159-57EAF12DDA24}">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -685,301 +680,235 @@
       <c r="C1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>36</v>
       </c>
       <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>21</v>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" t="s">
         <v>64</v>
       </c>
     </row>
@@ -989,7 +918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">

</xml_diff>